<commit_message>
DDT using Excel File & Cucumbar simple report
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/HrmsTestData.xlsx
+++ b/src/test/resources/testdata/HrmsTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fadwaazeroual/eclipse-workspace/HrmsFramework/src/test/resources/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fadwaazeroual/eclipse-workspace/Hrms/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9E6C44-A736-7345-9B8C-F78280EF0B4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D65ED0-DC75-9746-859B-BDF52E58A102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="1480" windowWidth="21900" windowHeight="13440" activeTab="1" xr2:uid="{732982CE-BAA9-2440-A2CD-1EC8CAB6B826}"/>
+    <workbookView xWindow="3620" yWindow="1480" windowWidth="21900" windowHeight="13440" xr2:uid="{732982CE-BAA9-2440-A2CD-1EC8CAB6B826}"/>
   </bookViews>
   <sheets>
     <sheet name="EmployeeLoginCredentials" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>FirstName</t>
   </si>
@@ -101,16 +101,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -163,12 +156,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,20 +475,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A06F2E9-E9A4-0845-B2E1-10FC177361B1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.5" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="17.5" style="1"/>
-    <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="17.5" style="1"/>
+    <col min="1" max="3" width="21.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
-  <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -505,70 +554,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED298BA-B6FA-9646-8536-3B99BAE3787B}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="16.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="34.5" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="3" width="16.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -587,28 +636,28 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="28.83203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="48" style="4" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="24.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="48" style="3" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>